<commit_message>
Updating Review sheet with all comments contains "3/2/2020" Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Review point</t>
   </si>
@@ -110,7 +110,73 @@
     <t xml:space="preserve">In requirement  Req_PO1_DGC_CYRS_005_V01 the ON/OFF operation is done using 2 switches while in SIQ sheet it's just one switch </t>
   </si>
   <si>
-    <t>28/1/2021</t>
+    <t>Acceptance</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Mali 3/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>28/1/2020</t>
+  </si>
+  <si>
+    <t>In requirement  Req_PO1_DGC_CYRS_005_V01 : Remove this part
+" If the LCD is off"</t>
+  </si>
+  <si>
+    <t>Document still in PDF format also Status still drat while it should be proposed as it's under review now</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In 1.2 version change history add the following comment "Fixing HSI requirement by replacing </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CYRS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> HSI</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -162,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -182,11 +248,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="36">
     <dxf>
       <font>
         <condense val="0"/>
@@ -215,13 +287,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -232,8 +297,199 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -605,10 +861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,11 +872,12 @@
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -634,13 +891,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="75">
+    <row r="2" spans="1:7" ht="75">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -653,13 +913,19 @@
       <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="45">
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="45">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
@@ -670,141 +936,198 @@
       <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45">
+      <c r="A4" s="8">
+        <v>43892</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="8">
+        <v>43892</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="5"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="E6" s="5"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="5"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="E9" s="2"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11" s="1"/>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="2:4">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="2:5">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="2:4">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="2:4">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="2:5">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="2:4">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="2:5">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="2:5">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="2:5">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="2:4">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="2:5">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E9">
-    <cfRule type="containsText" dxfId="8" priority="22" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="23" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="24" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E9">
+  <conditionalFormatting sqref="E2:E3">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9">
       <formula1>"Open, Closed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+      <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -814,10 +1137,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -826,11 +1149,12 @@
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="90.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -844,13 +1168,16 @@
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="60">
+    <row r="2" spans="1:7" ht="60">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -863,11 +1190,17 @@
       <c r="D2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30">
+      <c r="E2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -880,27 +1213,145 @@
       <c r="D3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="8">
+        <v>43892</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" ht="30">
+      <c r="A5" s="8">
+        <v>43892</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="E8" s="2"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="5:5">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="5:5">
+      <c r="E22" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F4">
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",E2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",E2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
+      <formula1>"Open, Closed"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
-      <formula1>"Open, Closed"</formula1>
+      <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Rebased SRS branch - Updated SRS document to v1.2
Signed-off-by: MinaH94 <mina.helmi.94@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CYRS review" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>Review point</t>
   </si>
@@ -178,12 +178,18 @@
       <t>"</t>
     </r>
   </si>
+  <si>
+    <t>Mali 6/2/2020: Point is reviewed and closed</t>
+  </si>
+  <si>
+    <t>Mali 6/2/2020: Point still open</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -258,7 +264,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="30">
     <dxf>
       <font>
         <condense val="0"/>
@@ -280,6 +286,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
@@ -299,6 +310,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <condense val="0"/>
         <extend val="0"/>
         <color rgb="FF9C0006"/>
@@ -344,13 +360,6 @@
       <font>
         <condense val="0"/>
         <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -361,7 +370,114 @@
     </dxf>
     <dxf>
       <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
       </font>
     </dxf>
     <dxf>
@@ -463,7 +579,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -495,10 +611,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +645,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -706,24 +820,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="59" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -746,7 +860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="75">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -769,7 +883,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="45">
       <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
@@ -792,7 +906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45">
       <c r="A4" s="8">
         <v>43892</v>
       </c>
@@ -809,11 +923,13 @@
         <v>17</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="8">
         <v>43892</v>
       </c>
@@ -830,11 +946,13 @@
         <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
@@ -843,7 +961,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -851,7 +969,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" s="1"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -859,7 +977,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" s="1"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -867,86 +985,86 @@
       <c r="E9" s="2"/>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
@@ -954,37 +1072,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F9">
-    <cfRule type="containsText" dxfId="16" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1002,25 +1120,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1043,7 +1161,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="60">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1066,7 +1184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1089,7 +1207,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="8">
         <v>43892</v>
       </c>
@@ -1102,13 +1220,17 @@
       <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30">
       <c r="A5" s="8">
         <v>43892</v>
       </c>
@@ -1121,99 +1243,130 @@
       <c r="D5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5">
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5">
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5">
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5">
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5">
       <c r="E22" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+      <formula>"Rejected"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+      <formula>"Accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
       <formula1>"Open, Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>"Accepted, Rejected"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Release HSI & CYRS Signed-off-by: MMohamedAli74 <mmohamedali74@gmail.com>
</commit_message>
<xml_diff>
--- a/Input documents/Review.xlsx
+++ b/Input documents/Review.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
   <si>
     <t>Review point</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Point status</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>Document</t>
@@ -264,7 +261,55 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -824,7 +869,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -845,65 +890,65 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="75">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45">
       <c r="A3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="45">
@@ -914,19 +959,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30">
@@ -937,19 +982,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1072,37 +1117,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F9">
-    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="6" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1124,7 +1169,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1146,65 +1191,65 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="30">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30">
@@ -1215,19 +1260,19 @@
         <v>3</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>22</v>
-      </c>
       <c r="G4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30">
@@ -1238,19 +1283,19 @@
         <v>3</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1306,60 +1351,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F4">
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="26" priority="22" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="25" priority="23" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E3">
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="20" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="21" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="9" operator="containsText" text="Closed">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Closed">
       <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="Open">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Open">
       <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="13" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"Rejected"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
       <formula>"Accepted"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="Closed">
+      <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="Open">
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Closed">
-      <formula>NOT(ISERROR(SEARCH("Closed",F4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Closed",F5)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Open">
-      <formula>NOT(ISERROR(SEARCH("Open",F4)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Open",F5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>